<commit_message>
Update Python.xlsx with new data
</commit_message>
<xml_diff>
--- a/Python.xlsx
+++ b/Python.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Python Training Plan"/>
@@ -561,13 +561,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -812,7 +812,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,7 +869,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,8 +907,8 @@
     <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -929,7 +929,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,7 +1235,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="42"/>
       <c r="B21" s="9" t="s">
         <v>123</v>
@@ -1529,7 +1529,7 @@
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="32.25">
       <c r="A29" s="42"/>
       <c r="B29" s="9" t="s">
         <v>137</v>
@@ -1774,7 +1774,7 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1818,7 +1818,7 @@
       </c>
       <c r="D3" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="24"/>
       <c r="B4" s="27"/>
       <c r="C4" s="19" t="s">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
         <v>70</v>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="D18" s="39"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="28"/>
       <c r="B19" s="21" t="s">
         <v>87</v>

</xml_diff>